<commit_message>
feat: import book 🔥
Kini dengan memilih jurusan terlebih dahulu
</commit_message>
<xml_diff>
--- a/public/template/import-books.xlsx
+++ b/public/template/import-books.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
-  <si>
-    <t xml:space="preserve">Major</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -43,22 +40,19 @@
     <t xml:space="preserve">Suplement</t>
   </si>
   <si>
-    <t xml:space="preserve">Umum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Judul Buku Akutansi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10001</t>
+    <t xml:space="preserve">Summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judul Buku Akutansi 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10010</t>
   </si>
   <si>
     <t xml:space="preserve">Name Penulis</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akutansi</t>
+    <t xml:space="preserve">Lorem Ipsum</t>
   </si>
   <si>
     <t xml:space="preserve">Judul Buku Ilmu Komunikasi</t>
@@ -67,9 +61,6 @@
     <t xml:space="preserve">10002</t>
   </si>
   <si>
-    <t xml:space="preserve">Ilmu Komunikasi</t>
-  </si>
-  <si>
     <t xml:space="preserve">Judul Buku Manajemen</t>
   </si>
   <si>
@@ -79,9 +70,6 @@
     <t xml:space="preserve">CD</t>
   </si>
   <si>
-    <t xml:space="preserve">Manajemen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Judul Buku Sastra Inggris</t>
   </si>
   <si>
@@ -91,27 +79,18 @@
     <t xml:space="preserve">DVD</t>
   </si>
   <si>
-    <t xml:space="preserve">Sastra Inggris</t>
-  </si>
-  <si>
     <t xml:space="preserve">Judul Buku Teknik Elektro</t>
   </si>
   <si>
     <t xml:space="preserve">10005</t>
   </si>
   <si>
-    <t xml:space="preserve">Teknik Elektro</t>
-  </si>
-  <si>
     <t xml:space="preserve">Judul Buku Informatika</t>
   </si>
   <si>
     <t xml:space="preserve">10006</t>
   </si>
   <si>
-    <t xml:space="preserve">Teknik Informatika</t>
-  </si>
-  <si>
     <t xml:space="preserve">Judul Buku Teknik Mesin</t>
   </si>
   <si>
@@ -121,16 +100,10 @@
     <t xml:space="preserve">Kalender</t>
   </si>
   <si>
-    <t xml:space="preserve">Teknik Mesin</t>
-  </si>
-  <si>
     <t xml:space="preserve">Judul Buku Teknik Sipil</t>
   </si>
   <si>
     <t xml:space="preserve">10008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teknik Sipil</t>
   </si>
   <si>
     <t xml:space="preserve">Judul Buku Umum</t>
@@ -147,7 +120,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -169,13 +142,27 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFEEEEEE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2A6099"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -212,13 +199,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -234,6 +229,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF2A6099"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -245,39 +300,39 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="46.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -285,207 +340,165 @@
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>95000</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>95000</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>10</v>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2001</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>2001</v>
-      </c>
-      <c r="F3" s="0" t="n">
         <v>95500</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>96000</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>2002</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>96000</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2003</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>2003</v>
-      </c>
-      <c r="F5" s="0" t="n">
         <v>96500</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>22</v>
+      <c r="F5" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>2004</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>2004</v>
-      </c>
-      <c r="F6" s="0" t="n">
         <v>97000</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2005</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>2005</v>
-      </c>
-      <c r="F7" s="0" t="n">
         <v>97500</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2006</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>2006</v>
-      </c>
-      <c r="F8" s="0" t="n">
         <v>98000</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>32</v>
+      <c r="F8" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2007</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>2007</v>
-      </c>
-      <c r="F9" s="0" t="n">
         <v>98500</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2008</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>2008</v>
-      </c>
-      <c r="F10" s="0" t="n">
         <v>99000</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>